<commit_message>
NOTE FILES - modified description of columns for search
</commit_message>
<xml_diff>
--- a/kategorie_temat_typovych_reseni.XLSX
+++ b/kategorie_temat_typovych_reseni.XLSX
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="1860" windowWidth="21600" windowHeight="11385" activeTab="2"/>
+    <workbookView xWindow="29820" yWindow="1860" windowWidth="21600" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kategorie_temat" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
   <si>
     <t>Nakupování</t>
   </si>
@@ -387,6 +387,36 @@
   </si>
   <si>
     <t>Snížení nákladů na Odpadové Hospodářství</t>
+  </si>
+  <si>
+    <t>column id</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
@@ -517,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +612,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -854,7 +890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3997,19 +4033,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>118</v>
       </c>
@@ -4017,189 +4054,261 @@
       <c r="C1" s="23" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C24" t="s">
         <v>90</v>
+      </c>
+      <c r="D24" s="27">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4212,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>